<commit_message>
Finally all bugs fixed
</commit_message>
<xml_diff>
--- a/ORCID-FIL.xlsx
+++ b/ORCID-FIL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marko.p.milovanovic/PycharmProjects/parser/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFF5EA7E-FC95-1843-87C1-1851B4F7F324}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6634EDB-23D5-C340-970E-2571920B1AED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16340" yWindow="3080" windowWidth="16980" windowHeight="17960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ORCId" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1267" uniqueCount="1075">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1280" uniqueCount="1088">
   <si>
     <t>Име</t>
   </si>
@@ -3395,12 +3395,51 @@
   <si>
     <t>0000-0003-1494-9390</t>
   </si>
+  <si>
+    <t>Ðorđević</t>
+  </si>
+  <si>
+    <t>Danijela</t>
+  </si>
+  <si>
+    <t>Vesić Pavlović</t>
+  </si>
+  <si>
+    <t>Tijana</t>
+  </si>
+  <si>
+    <t>0000-0002-8804-4037</t>
+  </si>
+  <si>
+    <t>0000-0001-5786-975X</t>
+  </si>
+  <si>
+    <t>Milošević</t>
+  </si>
+  <si>
+    <t>Ivan</t>
+  </si>
+  <si>
+    <t>0009-0005-7415-2300</t>
+  </si>
+  <si>
+    <t>Michael</t>
+  </si>
+  <si>
+    <t>McAteer</t>
+  </si>
+  <si>
+    <t>0009-0009-0551-563X</t>
+  </si>
+  <si>
+    <t>https://orcid.org/0009-0009-0551-563X</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="49">
+  <fonts count="50">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -3715,6 +3754,14 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -3745,10 +3792,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3813,8 +3861,10 @@
     </xf>
     <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4032,10 +4082,10 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AA297"/>
+  <dimension ref="A1:AA301"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="D71" sqref="D71"/>
+    <sheetView tabSelected="1" topLeftCell="A281" workbookViewId="0">
+      <selection activeCell="E307" sqref="E307"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -8700,6 +8750,53 @@
       </c>
       <c r="E297" s="21" t="s">
         <v>1071</v>
+      </c>
+    </row>
+    <row r="298" spans="2:5" ht="15.75" customHeight="1">
+      <c r="B298" s="46" t="s">
+        <v>1076</v>
+      </c>
+      <c r="C298" t="s">
+        <v>1075</v>
+      </c>
+      <c r="D298" t="s">
+        <v>1079</v>
+      </c>
+    </row>
+    <row r="299" spans="2:5" ht="15.75" customHeight="1">
+      <c r="B299" t="s">
+        <v>1078</v>
+      </c>
+      <c r="C299" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D299" t="s">
+        <v>1080</v>
+      </c>
+    </row>
+    <row r="300" spans="2:5" ht="15.75" customHeight="1">
+      <c r="B300" t="s">
+        <v>1082</v>
+      </c>
+      <c r="C300" t="s">
+        <v>1081</v>
+      </c>
+      <c r="D300" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="301" spans="2:5" ht="15.75" customHeight="1">
+      <c r="B301" s="46" t="s">
+        <v>1084</v>
+      </c>
+      <c r="C301" s="46" t="s">
+        <v>1085</v>
+      </c>
+      <c r="D301" s="46" t="s">
+        <v>1086</v>
+      </c>
+      <c r="E301" s="48" t="s">
+        <v>1087</v>
       </c>
     </row>
   </sheetData>
@@ -8897,6 +8994,7 @@
     <hyperlink ref="E296" r:id="rId191" xr:uid="{00000000-0004-0000-0000-0000BF000000}"/>
     <hyperlink ref="E297" r:id="rId192" xr:uid="{00000000-0004-0000-0000-0000C0000000}"/>
     <hyperlink ref="E84" r:id="rId193" xr:uid="{5F8AB1D8-7A93-E544-84F8-48799EE26CC8}"/>
+    <hyperlink ref="E301" r:id="rId194" xr:uid="{0B8C6C9E-50D0-1A41-A066-81EF12902922}"/>
   </hyperlinks>
   <printOptions horizontalCentered="1" gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>